<commit_message>
added top pk tables
</commit_message>
<xml_diff>
--- a/paper_elements/tables/tables.xlsx
+++ b/paper_elements/tables/tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61e649324136aa03/classes/COS484/cos 484 final project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafmos/cos484proj/paper_elements/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{EAF74589-7120-AA4A-ACED-76CB4084B0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E18DE6DD-84FB-4144-BCA6-659D21BB16D1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E200412-A2C4-F44C-B3EC-F8D268C5BE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="640" windowWidth="50880" windowHeight="26440" xr2:uid="{09FD0FEC-C134-094E-B1D4-F8BCD6F1B239}"/>
+    <workbookView xWindow="10620" yWindow="1040" windowWidth="25240" windowHeight="20640" xr2:uid="{09FD0FEC-C134-094E-B1D4-F8BCD6F1B239}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -615,6 +615,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -630,11 +635,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0537EC-BDB2-F348-86BC-6ACE3874E2B0}">
   <dimension ref="B2:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -986,33 +986,33 @@
       </c>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="38" t="s">
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="35" t="s">
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
-      <c r="V3" s="36"/>
-      <c r="W3" s="37"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="42"/>
     </row>
     <row r="4" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
@@ -1529,33 +1529,33 @@
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="38" t="s">
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="35" t="s">
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="R13" s="36"/>
-      <c r="S13" s="36"/>
-      <c r="T13" s="36"/>
-      <c r="U13" s="36"/>
-      <c r="V13" s="36"/>
-      <c r="W13" s="37"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="42"/>
     </row>
     <row r="14" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
@@ -1626,175 +1626,355 @@
       <c r="B15" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="15" t="e">
+      <c r="C15" s="13">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="D15" s="14">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="F15" s="14">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="G15" s="14">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="H15" s="14">
+        <v>0.83</v>
+      </c>
+      <c r="I15" s="15">
         <f>AVERAGE(C15:H15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="18" t="e">
+        <v>0.90316666666666678</v>
+      </c>
+      <c r="J15" s="16">
+        <v>0.96</v>
+      </c>
+      <c r="K15" s="17">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="L15" s="17">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="M15" s="17">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="N15" s="17">
+        <v>0.8</v>
+      </c>
+      <c r="O15" s="17">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="P15" s="18">
         <f>AVERAGE(J15:O15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
-      <c r="U15" s="17"/>
-      <c r="V15" s="17"/>
-      <c r="W15" s="19" t="e">
+        <v>0.88266666666666671</v>
+      </c>
+      <c r="Q15" s="16">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="R15" s="17">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="S15" s="17">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="T15" s="17">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="U15" s="17">
+        <v>0.97</v>
+      </c>
+      <c r="V15" s="17">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="W15" s="19">
         <f>AVERAGE(Q15:V15)</f>
-        <v>#DIV/0!</v>
+        <v>0.97366666666666657</v>
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="15" t="e">
+      <c r="C16" s="20">
+        <v>0.8</v>
+      </c>
+      <c r="D16" s="21">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="E16" s="21">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="F16" s="21">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="G16" s="21">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="H16" s="21">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="I16" s="15">
         <f>AVERAGE(C16:H16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J16" s="20"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="22" t="e">
+        <v>0.76316666666666666</v>
+      </c>
+      <c r="J16" s="20">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="K16" s="21">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="L16" s="21">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="M16" s="21">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="N16" s="21">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="O16" s="21">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="P16" s="22">
         <f>AVERAGE(J16:O16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21"/>
-      <c r="W16" s="23" t="e">
+        <v>0.80149999999999999</v>
+      </c>
+      <c r="Q16" s="20">
+        <v>0.875</v>
+      </c>
+      <c r="R16" s="21">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="S16" s="21">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="T16" s="21">
+        <v>0.83</v>
+      </c>
+      <c r="U16" s="21">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="V16" s="21">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="W16" s="23">
         <f>AVERAGE(Q16:V16)</f>
-        <v>#DIV/0!</v>
+        <v>0.83200000000000018</v>
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="15" t="e">
+      <c r="C17" s="20">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="D17" s="21">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="E17" s="21">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="F17" s="21">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="G17" s="21">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="H17" s="21">
+        <v>0.871</v>
+      </c>
+      <c r="I17" s="15">
         <f>AVERAGE(C17:H17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="22" t="e">
+        <v>0.92366666666666664</v>
+      </c>
+      <c r="J17" s="20">
+        <v>0.98</v>
+      </c>
+      <c r="K17" s="21">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="L17" s="21">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="M17" s="21">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="N17" s="21">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="O17" s="21">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="P17" s="22">
         <f>AVERAGE(J17:O17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="23" t="e">
+        <v>0.91349999999999998</v>
+      </c>
+      <c r="Q17" s="20">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="R17" s="21">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="S17" s="21">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="T17" s="21">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="U17" s="21">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="V17" s="21">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="W17" s="23">
         <f>AVERAGE(Q17:V17)</f>
-        <v>#DIV/0!</v>
+        <v>0.98050000000000004</v>
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="15" t="e">
+      <c r="C18" s="20">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="D18" s="21">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="E18" s="21">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="F18" s="21">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="G18" s="21">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="H18" s="21">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="I18" s="15">
         <f>AVERAGE(C18:H18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="22" t="e">
+        <v>0.53233333333333344</v>
+      </c>
+      <c r="J18" s="20">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="K18" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="L18" s="21">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="M18" s="21">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="N18" s="21">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="O18" s="21">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="P18" s="22">
         <f>AVERAGE(J18:O18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="21"/>
-      <c r="V18" s="21"/>
-      <c r="W18" s="23" t="e">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="Q18" s="20">
+        <v>0.318</v>
+      </c>
+      <c r="R18" s="21">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="S18" s="21">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="T18" s="21">
+        <v>0.32</v>
+      </c>
+      <c r="U18" s="21">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="V18" s="21">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="W18" s="23">
         <f>AVERAGE(Q18:V18)</f>
-        <v>#DIV/0!</v>
+        <v>0.32616666666666666</v>
       </c>
     </row>
     <row r="19" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="26" t="e">
+      <c r="C19" s="24">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="D19" s="25">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="E19" s="25">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="F19" s="25">
+        <v>0.97</v>
+      </c>
+      <c r="G19" s="25">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="H19" s="25">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="I19" s="26">
         <f>AVERAGE(C19:H19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J19" s="24"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="25"/>
-      <c r="P19" s="27" t="e">
+        <v>0.97166666666666668</v>
+      </c>
+      <c r="J19" s="24">
+        <v>0.995</v>
+      </c>
+      <c r="K19" s="25">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="L19" s="25">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="M19" s="25">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="N19" s="25">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="O19" s="25">
+        <v>0.84</v>
+      </c>
+      <c r="P19" s="27">
         <f>AVERAGE(J19:O19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="29"/>
-      <c r="V19" s="29"/>
-      <c r="W19" s="30" t="e">
+        <v>0.92033333333333334</v>
+      </c>
+      <c r="Q19" s="28">
+        <v>0.995</v>
+      </c>
+      <c r="R19" s="29">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="S19" s="29">
+        <v>0.99</v>
+      </c>
+      <c r="T19" s="29">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="U19" s="29">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="V19" s="29">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="W19" s="30">
         <f>AVERAGE(Q19:V19)</f>
-        <v>#DIV/0!</v>
+        <v>0.97066666666666668</v>
       </c>
     </row>
     <row r="20" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1802,88 +1982,88 @@
         <v>19</v>
       </c>
       <c r="C20" s="31">
-        <f>C19-MAX(C15:C18)</f>
-        <v>0</v>
+        <f t="shared" ref="C20:W20" si="15">C19-MAX(C15:C18)</f>
+        <v>4.2000000000000037E-2</v>
       </c>
       <c r="D20" s="32">
-        <f>D19-MAX(D15:D18)</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>3.400000000000003E-2</v>
       </c>
       <c r="E20" s="32">
-        <f>E19-MAX(E15:E18)</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>2.9000000000000026E-2</v>
       </c>
       <c r="F20" s="32">
-        <f>F19-MAX(F15:F18)</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>4.7999999999999932E-2</v>
       </c>
       <c r="G20" s="32">
-        <f>G19-MAX(G15:G18)</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>8.2999999999999963E-2</v>
       </c>
       <c r="H20" s="32">
-        <f>H19-MAX(H15:H18)</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="33" t="e">
-        <f>I19-MAX(I15:I18)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="15"/>
+        <v>5.2000000000000046E-2</v>
+      </c>
+      <c r="I20" s="33">
+        <f t="shared" si="15"/>
+        <v>4.8000000000000043E-2</v>
       </c>
       <c r="J20" s="31">
-        <f>J19-MAX(J15:J18)</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>1.5000000000000013E-2</v>
       </c>
       <c r="K20" s="32">
-        <f>K19-MAX(K15:K18)</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>2.1000000000000019E-2</v>
       </c>
       <c r="L20" s="32">
-        <f>L19-MAX(L15:L18)</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>3.8000000000000034E-2</v>
       </c>
       <c r="M20" s="32">
-        <f>M19-MAX(M15:M18)</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>2.0000000000000018E-3</v>
       </c>
       <c r="N20" s="32">
-        <f>N19-MAX(N15:N18)</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>-2.399999999999991E-2</v>
       </c>
       <c r="O20" s="32">
-        <f>O19-MAX(O15:O18)</f>
-        <v>0</v>
-      </c>
-      <c r="P20" s="32" t="e">
-        <f>P19-MAX(P15:P18)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="15"/>
+        <v>-1.100000000000001E-2</v>
+      </c>
+      <c r="P20" s="32">
+        <f t="shared" si="15"/>
+        <v>6.8333333333333579E-3</v>
       </c>
       <c r="Q20" s="32">
-        <f>Q19-MAX(Q15:Q18)</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>4.0000000000000036E-3</v>
       </c>
       <c r="R20" s="32">
-        <f>R19-MAX(R15:R18)</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>7.0000000000000062E-3</v>
       </c>
       <c r="S20" s="32">
-        <f>S19-MAX(S15:S18)</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>5.0000000000000044E-3</v>
       </c>
       <c r="T20" s="32">
-        <f>T19-MAX(T15:T18)</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>-7.0000000000000062E-3</v>
       </c>
       <c r="U20" s="32">
-        <f>U19-MAX(U15:U18)</f>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>-3.5000000000000031E-2</v>
       </c>
       <c r="V20" s="32">
-        <f>V19-MAX(V15:V18)</f>
-        <v>0</v>
-      </c>
-      <c r="W20" s="34" t="e">
-        <f>W19-MAX(W15:W18)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="15"/>
+        <v>-3.2999999999999918E-2</v>
+      </c>
+      <c r="W20" s="34">
+        <f t="shared" si="15"/>
+        <v>-9.8333333333333606E-3</v>
       </c>
     </row>
     <row r="22" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1892,33 +2072,33 @@
       </c>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="38" t="s">
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="35" t="s">
+      <c r="K23" s="41"/>
+      <c r="L23" s="41"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="42"/>
+      <c r="Q23" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="R23" s="36"/>
-      <c r="S23" s="36"/>
-      <c r="T23" s="36"/>
-      <c r="U23" s="36"/>
-      <c r="V23" s="36"/>
-      <c r="W23" s="37"/>
+      <c r="R23" s="41"/>
+      <c r="S23" s="41"/>
+      <c r="T23" s="41"/>
+      <c r="U23" s="41"/>
+      <c r="V23" s="41"/>
+      <c r="W23" s="42"/>
     </row>
     <row r="24" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C24" s="5" t="s">
@@ -2345,87 +2525,87 @@
         <v>19</v>
       </c>
       <c r="C30" s="31">
-        <f>C29-MAX(C25:C28)</f>
+        <f t="shared" ref="C30:W30" si="16">C29-MAX(C25:C28)</f>
         <v>6.1999999999999944E-2</v>
       </c>
       <c r="D30" s="32">
-        <f>D29-MAX(D25:D28)</f>
+        <f t="shared" si="16"/>
         <v>4.1999999999999926E-2</v>
       </c>
       <c r="E30" s="32">
-        <f>E29-MAX(E25:E28)</f>
+        <f t="shared" si="16"/>
         <v>5.2000000000000046E-2</v>
       </c>
       <c r="F30" s="32">
-        <f>F29-MAX(F25:F28)</f>
+        <f t="shared" si="16"/>
         <v>7.3999999999999955E-2</v>
       </c>
       <c r="G30" s="32">
-        <f>G29-MAX(G25:G28)</f>
+        <f t="shared" si="16"/>
         <v>0.121</v>
       </c>
       <c r="H30" s="32">
-        <f>H29-MAX(H25:H28)</f>
+        <f t="shared" si="16"/>
         <v>-2.7999999999999914E-2</v>
       </c>
       <c r="I30" s="33">
-        <f>I29-MAX(I25:I28)</f>
+        <f t="shared" si="16"/>
         <v>5.3833333333333289E-2</v>
       </c>
       <c r="J30" s="31">
-        <f>J29-MAX(J25:J28)</f>
+        <f t="shared" si="16"/>
         <v>2.8000000000000025E-2</v>
       </c>
       <c r="K30" s="32">
-        <f>K29-MAX(K25:K28)</f>
+        <f t="shared" si="16"/>
         <v>3.8000000000000034E-2</v>
       </c>
       <c r="L30" s="32">
-        <f>L29-MAX(L25:L28)</f>
+        <f t="shared" si="16"/>
         <v>4.8999999999999932E-2</v>
       </c>
       <c r="M30" s="32">
-        <f>M29-MAX(M25:M28)</f>
+        <f t="shared" si="16"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="N30" s="32">
-        <f>N29-MAX(N25:N28)</f>
+        <f t="shared" si="16"/>
         <v>3.0000000000000027E-3</v>
       </c>
       <c r="O30" s="32">
-        <f>O29-MAX(O25:O28)</f>
+        <f t="shared" si="16"/>
         <v>-8.0000000000000071E-2</v>
       </c>
       <c r="P30" s="32">
-        <f>P29-MAX(P25:P28)</f>
+        <f t="shared" si="16"/>
         <v>9.6666666666666012E-3</v>
       </c>
       <c r="Q30" s="32">
-        <f>Q29-MAX(Q25:Q28)</f>
+        <f t="shared" si="16"/>
         <v>1.2000000000000011E-2</v>
       </c>
       <c r="R30" s="32">
-        <f>R29-MAX(R25:R28)</f>
+        <f t="shared" si="16"/>
         <v>1.8000000000000016E-2</v>
       </c>
       <c r="S30" s="32">
-        <f>S29-MAX(S25:S28)</f>
+        <f t="shared" si="16"/>
         <v>1.2000000000000011E-2</v>
       </c>
       <c r="T30" s="32">
-        <f>T29-MAX(T25:T28)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U30" s="32">
-        <f>U29-MAX(U25:U28)</f>
+        <f t="shared" si="16"/>
         <v>-3.7999999999999923E-2</v>
       </c>
       <c r="V30" s="32">
-        <f>V29-MAX(V25:V28)</f>
+        <f t="shared" si="16"/>
         <v>-6.0999999999999943E-2</v>
       </c>
       <c r="W30" s="34">
-        <f>W29-MAX(W25:W28)</f>
+        <f t="shared" si="16"/>
         <v>-9.5000000000000639E-3</v>
       </c>
     </row>
@@ -2435,18 +2615,18 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C33" s="38" t="s">
+      <c r="C33" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36" t="s">
+      <c r="D33" s="41"/>
+      <c r="E33" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36" t="s">
+      <c r="F33" s="41"/>
+      <c r="G33" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="37"/>
+      <c r="H33" s="42"/>
     </row>
     <row r="34" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
@@ -2472,25 +2652,25 @@
       <c r="B35" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="16" t="e">
+      <c r="C35" s="16">
         <f>main!I15</f>
-        <v>#DIV/0!</v>
+        <v>0.90316666666666678</v>
       </c>
       <c r="D35" s="18">
         <f>main!I25</f>
         <v>0.88149999999999995</v>
       </c>
-      <c r="E35" s="16" t="e">
+      <c r="E35" s="16">
         <f>main!P15</f>
-        <v>#DIV/0!</v>
+        <v>0.88266666666666671</v>
       </c>
       <c r="F35" s="19">
         <f>main!P25</f>
         <v>0.86299999999999999</v>
       </c>
-      <c r="G35" s="42" t="e">
+      <c r="G35" s="37">
         <f>main!W15</f>
-        <v>#DIV/0!</v>
+        <v>0.97366666666666657</v>
       </c>
       <c r="H35" s="19">
         <f>main!W25</f>
@@ -2501,25 +2681,25 @@
       <c r="B36" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="13" t="e">
+      <c r="C36" s="13">
         <f>main!I16</f>
-        <v>#DIV/0!</v>
+        <v>0.76316666666666666</v>
       </c>
       <c r="D36" s="22">
         <f>main!I26</f>
         <v>0.76266666666666671</v>
       </c>
-      <c r="E36" s="13" t="e">
+      <c r="E36" s="13">
         <f>main!P16</f>
-        <v>#DIV/0!</v>
+        <v>0.80149999999999999</v>
       </c>
       <c r="F36" s="23">
         <f>main!P26</f>
         <v>0.79933333333333334</v>
       </c>
-      <c r="G36" s="43" t="e">
+      <c r="G36" s="38">
         <f>main!W16</f>
-        <v>#DIV/0!</v>
+        <v>0.83200000000000018</v>
       </c>
       <c r="H36" s="23">
         <f>main!W26</f>
@@ -2530,25 +2710,25 @@
       <c r="B37" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="13" t="e">
+      <c r="C37" s="13">
         <f>main!I17</f>
-        <v>#DIV/0!</v>
+        <v>0.92366666666666664</v>
       </c>
       <c r="D37" s="22">
         <f>main!I27</f>
         <v>0.91283333333333339</v>
       </c>
-      <c r="E37" s="13" t="e">
+      <c r="E37" s="13">
         <f>main!P17</f>
-        <v>#DIV/0!</v>
+        <v>0.91349999999999998</v>
       </c>
       <c r="F37" s="23">
         <f>main!P27</f>
         <v>0.90483333333333338</v>
       </c>
-      <c r="G37" s="43" t="e">
+      <c r="G37" s="38">
         <f>main!W17</f>
-        <v>#DIV/0!</v>
+        <v>0.98050000000000004</v>
       </c>
       <c r="H37" s="23">
         <f>main!W27</f>
@@ -2559,25 +2739,25 @@
       <c r="B38" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="13" t="e">
+      <c r="C38" s="13">
         <f>main!I18</f>
-        <v>#DIV/0!</v>
+        <v>0.53233333333333344</v>
       </c>
       <c r="D38" s="22">
         <f>main!I28</f>
         <v>0.54633333333333345</v>
       </c>
-      <c r="E38" s="13" t="e">
+      <c r="E38" s="13">
         <f>main!P18</f>
-        <v>#DIV/0!</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="F38" s="23">
         <f>main!P28</f>
         <v>0.54283333333333328</v>
       </c>
-      <c r="G38" s="43" t="e">
+      <c r="G38" s="38">
         <f>main!W18</f>
-        <v>#DIV/0!</v>
+        <v>0.32616666666666666</v>
       </c>
       <c r="H38" s="23">
         <f>main!W28</f>
@@ -2588,25 +2768,25 @@
       <c r="B39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="40" t="e">
+      <c r="C39" s="35">
         <f>main!I19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D39" s="41">
+        <v>0.97166666666666668</v>
+      </c>
+      <c r="D39" s="36">
         <f>main!I29</f>
         <v>0.96666666666666667</v>
       </c>
-      <c r="E39" s="40" t="e">
+      <c r="E39" s="35">
         <f>main!P19</f>
-        <v>#DIV/0!</v>
+        <v>0.92033333333333334</v>
       </c>
       <c r="F39" s="30">
         <f>main!P29</f>
         <v>0.91449999999999998</v>
       </c>
-      <c r="G39" s="44" t="e">
+      <c r="G39" s="39">
         <f>main!W19</f>
-        <v>#DIV/0!</v>
+        <v>0.97066666666666668</v>
       </c>
       <c r="H39" s="30">
         <f>main!W29</f>

</xml_diff>